<commit_message>
[ELAB-429] added first section of explaining the Demo
</commit_message>
<xml_diff>
--- a/data/cross-browser Metastudie/cross-browser_Metastudie.xlsx
+++ b/data/cross-browser Metastudie/cross-browser_Metastudie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\cross-browser Metastudie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540A544C-6B12-4F95-9EF3-7A0AF44DD9A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE8AFB2-03FF-4CDC-BBC7-82B3B86537FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{54D5DEE8-7292-4CF4-A1C3-548CC96A1DD8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Jahr</t>
   </si>
@@ -63,7 +63,10 @@
     <t>Treffer</t>
   </si>
   <si>
-    <t>2020 (*2)</t>
+    <t>2020 (14.01.21)</t>
+  </si>
+  <si>
+    <t>2020 (21.12.20)</t>
   </si>
 </sst>
 </file>
@@ -418,22 +421,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE6ED51-2386-4F7B-807A-8C98984AFD18}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -442,7 +445,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -459,7 +462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -479,7 +482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -499,7 +502,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -519,7 +522,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -539,7 +542,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -559,7 +562,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -579,7 +582,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -599,9 +602,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>313</v>
@@ -617,6 +620,26 @@
       </c>
       <c r="F10">
         <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>335</v>
+      </c>
+      <c r="C11">
+        <v>62</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>146</v>
+      </c>
+      <c r="F11">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>